<commit_message>
Syntax change, squash commit later or just ignore.
</commit_message>
<xml_diff>
--- a/files/CalorieCount.xlsx
+++ b/files/CalorieCount.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aiswarya/Library/Mobile Documents/com~apple~CloudDocs/Career/PersonalWebpage/aiswarya-prasad.github.io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1105DE78-9C4A-7E4F-A0C8-B94B527B5CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399FAA94-2044-A34E-9C00-165AED624369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="15520" xr2:uid="{ACA7B0ED-6F5E-CC4C-BDE5-9936D6B17761}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculate" sheetId="1" r:id="rId1"/>
     <sheet name="Labels" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -507,7 +507,7 @@
   <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>